<commit_message>
atualizado dados do IHFA desde nov/2012
</commit_message>
<xml_diff>
--- a/output/ABSOLUTE_18422272000145.xlsx
+++ b/output/ABSOLUTE_18422272000145.xlsx
@@ -1351,10 +1351,10 @@
         <v>44165</v>
       </c>
       <c r="B88">
-        <v>1.395738</v>
+        <v>1.3982594</v>
       </c>
       <c r="C88">
-        <v>0.009250608028354534</v>
+        <v>0.0103127961654057</v>
       </c>
     </row>
   </sheetData>

</xml_diff>